<commit_message>
Allowed to read new .json to identify a subset of rivers, reducing the number of E. coli-like tracers to be modelled
</commit_message>
<xml_diff>
--- a/src/mitgcm_inputs/rbcs/Allegato_1_Capitolato_Tecnico_B32_B35_scarichi.xlsx
+++ b/src/mitgcm_inputs/rbcs/Allegato_1_Capitolato_Tecnico_B32_B35_scarichi.xlsx
@@ -2609,79 +2609,79 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="5" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2769,10 +2769,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0855195371324404"/>
-          <c:y val="0.041958041958042"/>
-          <c:w val="0.875564714274392"/>
-          <c:h val="0.869352869352869"/>
+          <c:x val="0.0855263157894737"/>
+          <c:y val="0.0419626998223801"/>
+          <c:w val="0.875475586556753"/>
+          <c:h val="0.869227353463588"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4368,7 +4368,7 @@
                   <c:v>13.5928</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.6915</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>13.2415</c:v>
@@ -4452,7 +4452,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.248</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -4509,7 +4509,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>11.2746</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>13.691</c:v>
@@ -4533,7 +4533,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>13.14344</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -4551,7 +4551,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>14.9987</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -5085,7 +5085,7 @@
                   <c:v>45.6941</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.6401</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>45.65372</c:v>
@@ -5169,7 +5169,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>44.32298</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -5226,7 +5226,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42.415</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>43.3771</c:v>
@@ -5250,7 +5250,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>41.23262</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
                   <c:v>0</c:v>
@@ -5268,7 +5268,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>42.00606</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>0</c:v>
@@ -5770,11 +5770,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2593572"/>
-        <c:axId val="50046594"/>
+        <c:axId val="57412454"/>
+        <c:axId val="50280043"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2593572"/>
+        <c:axId val="57412454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="19"/>
@@ -5818,12 +5818,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50046594"/>
+        <c:crossAx val="50280043"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50046594"/>
+        <c:axId val="50280043"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="46"/>
@@ -5867,7 +5867,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2593572"/>
+        <c:crossAx val="57412454"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5940,7 +5940,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1389960</xdr:colOff>
+      <xdr:colOff>1389600</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
@@ -5952,13 +5952,18 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="3472920" cy="360"/>
+          <a:ext cx="3472560" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
-          <a:gdLst/>
+          <a:gdLst>
+            <a:gd name="textAreaLeft" fmla="*/ 0 w 3472560"/>
+            <a:gd name="textAreaRight" fmla="*/ 3472920 w 3472560"/>
+            <a:gd name="textAreaTop" fmla="*/ 0 h 360"/>
+            <a:gd name="textAreaBottom" fmla="*/ 720 h 360"/>
+          </a:gdLst>
           <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:rect l="textAreaLeft" t="textAreaTop" r="textAreaRight" b="textAreaBottom"/>
           <a:pathLst>
             <a:path w="3030220" h="0">
               <a:moveTo>
@@ -5997,9 +6002,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>421560</xdr:colOff>
+      <xdr:colOff>421200</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6008,7 +6013,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13190040" y="534600"/>
-        <a:ext cx="4541760" cy="3242880"/>
+        <a:ext cx="4541400" cy="3242520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6203,8 +6208,8 @@
   </sheetPr>
   <dimension ref="A1:O238"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I58" activeCellId="0" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6296,12 +6301,12 @@
         <f aca="false">IF(I2&gt;0,E2)</f>
         <v>0</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="16" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="16" t="n">
         <f aca="false">COUNTIF(I:I,N2)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6340,7 +6345,7 @@
         <f aca="false">IF(I3&gt;0,E3)</f>
         <v>12.381</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="16" t="n">
         <v>2</v>
       </c>
       <c r="O3" s="16" t="n">
@@ -6384,7 +6389,7 @@
         <f aca="false">IF(I4&gt;0,E4)</f>
         <v>12.556</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="16" t="n">
         <v>3</v>
       </c>
       <c r="O4" s="16" t="n">
@@ -6425,7 +6430,7 @@
         <f aca="false">IF(I5&gt;0,E5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="16" t="n">
         <v>4</v>
       </c>
       <c r="O5" s="16" t="n">
@@ -6466,12 +6471,12 @@
         <f aca="false">IF(I6&gt;0,E6)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="16" t="n">
         <v>5</v>
       </c>
       <c r="O6" s="16" t="n">
         <f aca="false">COUNTIF(I:I,N6)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6513,12 +6518,12 @@
         <f aca="false">IF(I7&gt;0,E7)</f>
         <v>13.6915</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="16" t="n">
         <v>6</v>
       </c>
       <c r="O7" s="16" t="n">
         <f aca="false">COUNTIF(I:I,N7)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6557,7 +6562,7 @@
         <f aca="false">IF(I8&gt;0,E8)</f>
         <v>13.18995</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="16" t="n">
         <v>7</v>
       </c>
       <c r="O8" s="16" t="n">
@@ -6600,7 +6605,7 @@
       </c>
       <c r="O9" s="16" t="n">
         <f aca="false">SUM(O2:O8)</f>
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6668,19 +6673,13 @@
       <c r="H11" s="14" t="n">
         <v>62290</v>
       </c>
-      <c r="I11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="3" t="n">
-        <v>8</v>
-      </c>
       <c r="L11" s="17" t="n">
         <f aca="false">IF(I11&gt;0,D11)</f>
-        <v>45.6401</v>
+        <v>0</v>
       </c>
       <c r="M11" s="17" t="n">
         <f aca="false">IF(I11&gt;0,E11)</f>
-        <v>13.6915</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7647,16 +7646,13 @@
       <c r="H39" s="14" t="n">
         <v>56537</v>
       </c>
-      <c r="I39" s="3" t="n">
-        <v>6</v>
-      </c>
       <c r="L39" s="17" t="n">
         <f aca="false">IF(I39&gt;0,D39)</f>
-        <v>44.32298</v>
+        <v>0</v>
       </c>
       <c r="M39" s="17" t="n">
         <f aca="false">IF(I39&gt;0,E39)</f>
-        <v>9.248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8299,16 +8295,13 @@
       <c r="H58" s="14" t="n">
         <v>57584</v>
       </c>
-      <c r="I58" s="3" t="n">
-        <v>6</v>
-      </c>
       <c r="L58" s="17" t="n">
         <f aca="false">IF(I58&gt;0,D58)</f>
-        <v>42.415</v>
+        <v>0</v>
       </c>
       <c r="M58" s="17" t="n">
         <f aca="false">IF(I58&gt;0,E58)</f>
-        <v>11.2746</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8586,16 +8579,13 @@
       <c r="H66" s="14" t="n">
         <v>39867</v>
       </c>
-      <c r="I66" s="3" t="n">
-        <v>5</v>
-      </c>
       <c r="L66" s="17" t="n">
         <f aca="false">IF(I66&gt;0,D66)</f>
-        <v>41.23262</v>
+        <v>0</v>
       </c>
       <c r="M66" s="17" t="n">
         <f aca="false">IF(I66&gt;0,E66)</f>
-        <v>13.14344</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8793,16 +8783,13 @@
       <c r="H72" s="14" t="n">
         <v>34236</v>
       </c>
-      <c r="I72" s="3" t="n">
-        <v>5</v>
-      </c>
       <c r="L72" s="17" t="n">
         <f aca="false">IF(I72&gt;0,D72)</f>
-        <v>42.00606</v>
+        <v>0</v>
       </c>
       <c r="M72" s="17" t="n">
         <f aca="false">IF(I72&gt;0,E72)</f>
-        <v>14.9987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>